<commit_message>
Adding old and new security baselines.  Updated b1903 baseline to recent September changes.
</commit_message>
<xml_diff>
--- a/Microsoft Windows Security Baseline/Windows 10 Version 1903/Windows 10 Version 1903 Security Baseline Policies.xlsx
+++ b/Microsoft Windows Security Baseline/Windows 10 Version 1903/Windows 10 Version 1903 Security Baseline Policies.xlsx
@@ -1,17 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_Development\LGPO\Microsoft Windows Security Baseline\Windows 10 Version 1903\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
   </bookViews>
   <sheets>
     <sheet name="Computer" sheetId="1" r:id="rId1"/>
     <sheet name="User" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Computer!$A$1:$E$204</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Computer!$A$1:$E$203</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">User!$A$1:$E$4</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
@@ -24,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1037" uniqueCount="637">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1032" uniqueCount="633">
   <si>
     <t>Policy Path</t>
   </si>
@@ -628,21 +633,6 @@
 --  "Authenticated" allows only authenticated RPC Clients (per the definition above) to connect to RPC Servers running on the machine on which the policy setting is applied. Exemptions are granted to interfaces that have requested them.
 --  "Authenticated without exceptions" allows only authenticated RPC Clients (per the definition above) to connect to RPC Servers running on the machine on which the policy setting is applied.  No exceptions are allowed.
 Note: This policy setting will not be applied until the system is rebooted.</t>
-  </si>
-  <si>
-    <t>System\Service Control Manager Settings\Security Settings</t>
-  </si>
-  <si>
-    <t>Enable svchost.exe mitigation options</t>
-  </si>
-  <si>
-    <t>HKLM\System\CurrentControlSet\Control\SCMConfig!EnableSvchostMitigationPolicy</t>
-  </si>
-  <si>
-    <t>This policy setting enables process mitigation options on svchost.exe processes.
-If you enable this policy setting, built-in system services hosted in svchost.exe processes will have stricter security policies enabled on them.
-This includes a policy requiring all binaries loaded in these processes to be signed by microsoft, as well as a policy disallowing dynamically-generated code.
-If you disable or do not configure this policy setting, these stricter security settings will not be applied.</t>
   </si>
   <si>
     <t>Windows Components\App Privacy</t>
@@ -2615,7 +2605,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2950,7 +2940,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2958,12 +2948,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E204"/>
+  <dimension ref="A1:E203"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
       <selection activeCell="A2" sqref="A2"/>
-      <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
+      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.4" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2984,7 +2974,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>636</v>
+        <v>632</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>2</v>
@@ -3630,24 +3620,24 @@
         <v>147</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>6</v>
+        <v>148</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="E39" s="5" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>152</v>
+        <v>6</v>
       </c>
       <c r="D40" s="4" t="s">
         <v>153</v>
@@ -3675,13 +3665,13 @@
     </row>
     <row r="42" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="B42" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="B42" s="4" t="s">
+      <c r="C42" s="4" t="s">
         <v>160</v>
-      </c>
-      <c r="C42" s="4" t="s">
-        <v>6</v>
       </c>
       <c r="D42" s="4" t="s">
         <v>161</v>
@@ -3692,7 +3682,7 @@
     </row>
     <row r="43" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="B43" s="4" t="s">
         <v>163</v>
@@ -3709,13 +3699,13 @@
     </row>
     <row r="44" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
-        <v>159</v>
+        <v>167</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>168</v>
+        <v>6</v>
       </c>
       <c r="D44" s="4" t="s">
         <v>169</v>
@@ -3759,33 +3749,33 @@
       </c>
     </row>
     <row r="47" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="4" t="s">
+      <c r="A47" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="B47" s="4" t="s">
+      <c r="B47" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="C47" s="4" t="s">
+      <c r="C47" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="D47" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="E47" s="5" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="C48" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D47" s="4" t="s">
-        <v>181</v>
-      </c>
-      <c r="E47" s="5" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="C48" s="5" t="s">
-        <v>185</v>
-      </c>
-      <c r="D48" s="5" t="s">
+      <c r="D48" s="4" t="s">
         <v>186</v>
       </c>
       <c r="E48" s="5" t="s">
@@ -3800,7 +3790,7 @@
         <v>189</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="D49" s="4" t="s">
         <v>190</v>
@@ -3816,8 +3806,8 @@
       <c r="B50" s="4" t="s">
         <v>193</v>
       </c>
-      <c r="C50" s="4" t="s">
-        <v>25</v>
+      <c r="C50" s="4">
+        <v>32768</v>
       </c>
       <c r="D50" s="4" t="s">
         <v>194</v>
@@ -3831,63 +3821,63 @@
         <v>196</v>
       </c>
       <c r="B51" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="C51" s="4">
+        <v>196608</v>
+      </c>
+      <c r="D51" s="4" t="s">
         <v>197</v>
       </c>
-      <c r="C51" s="4">
-        <v>32768</v>
-      </c>
-      <c r="D51" s="4" t="s">
+      <c r="E51" s="5" t="s">
         <v>198</v>
-      </c>
-      <c r="E51" s="5" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="52" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="B52" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="C52" s="4">
+        <v>32768</v>
+      </c>
+      <c r="D52" s="4" t="s">
         <v>200</v>
       </c>
-      <c r="B52" s="4" t="s">
-        <v>197</v>
-      </c>
-      <c r="C52" s="4">
-        <v>196608</v>
-      </c>
-      <c r="D52" s="4" t="s">
+      <c r="E52" s="5" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="E52" s="5" t="s">
+      <c r="B53" s="1" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="53" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="4" t="s">
+      <c r="C53" s="5" t="s">
         <v>203</v>
       </c>
-      <c r="B53" s="4" t="s">
-        <v>197</v>
-      </c>
-      <c r="C53" s="4">
-        <v>32768</v>
-      </c>
-      <c r="D53" s="4" t="s">
+      <c r="D53" s="5" t="s">
         <v>204</v>
       </c>
       <c r="E53" s="5" t="s">
-        <v>199</v>
+        <v>205</v>
       </c>
     </row>
     <row r="54" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="C54" s="5" t="s">
         <v>207</v>
       </c>
-      <c r="D54" s="5" t="s">
+      <c r="C54" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D54" s="4" t="s">
         <v>208</v>
       </c>
       <c r="E54" s="5" t="s">
@@ -3896,30 +3886,30 @@
     </row>
     <row r="55" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="B55" s="1" t="s">
         <v>210</v>
-      </c>
-      <c r="B55" s="1" t="s">
-        <v>211</v>
       </c>
       <c r="C55" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D55" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="E55" s="5" t="s">
         <v>212</v>
       </c>
-      <c r="E55" s="5" t="s">
+    </row>
+    <row r="56" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="B56" s="4" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="56" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="B56" s="1" t="s">
+      <c r="C56" s="4" t="s">
         <v>214</v>
-      </c>
-      <c r="C56" s="4" t="s">
-        <v>6</v>
       </c>
       <c r="D56" s="4" t="s">
         <v>215</v>
@@ -3929,133 +3919,133 @@
       </c>
     </row>
     <row r="57" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="4" t="s">
-        <v>210</v>
-      </c>
-      <c r="B57" s="4" t="s">
+      <c r="A57" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="B57" s="1" t="s">
         <v>217</v>
       </c>
       <c r="C57" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D57" s="4" t="s">
         <v>218</v>
       </c>
-      <c r="D57" s="4" t="s">
+      <c r="E57" s="5" t="s">
         <v>219</v>
       </c>
-      <c r="E57" s="5" t="s">
+    </row>
+    <row r="58" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="B58" s="4" t="s">
         <v>220</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="B58" s="1" t="s">
-        <v>221</v>
       </c>
       <c r="C58" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D58" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="E58" s="5" t="s">
         <v>222</v>
-      </c>
-      <c r="E58" s="5" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="59" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C59" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D59" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="E59" s="5" t="s">
         <v>225</v>
-      </c>
-      <c r="E59" s="5" t="s">
-        <v>226</v>
       </c>
     </row>
     <row r="60" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C60" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D60" s="4" t="s">
+        <v>227</v>
+      </c>
+      <c r="E60" s="5" t="s">
         <v>228</v>
-      </c>
-      <c r="E60" s="5" t="s">
-        <v>229</v>
       </c>
     </row>
     <row r="61" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C61" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D61" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="E61" s="5" t="s">
         <v>231</v>
-      </c>
-      <c r="E61" s="5" t="s">
-        <v>232</v>
       </c>
     </row>
     <row r="62" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C62" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D62" s="4" t="s">
+        <v>233</v>
+      </c>
+      <c r="E62" s="5" t="s">
         <v>234</v>
-      </c>
-      <c r="E62" s="5" t="s">
-        <v>235</v>
       </c>
     </row>
     <row r="63" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="4" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="B63" s="4" t="s">
+        <v>235</v>
+      </c>
+      <c r="C63" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D63" s="4" t="s">
         <v>236</v>
       </c>
-      <c r="C63" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D63" s="4" t="s">
+      <c r="E63" s="5" t="s">
         <v>237</v>
-      </c>
-      <c r="E63" s="5" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="64" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="4" t="s">
-        <v>210</v>
+        <v>238</v>
       </c>
       <c r="B64" s="4" t="s">
         <v>239</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="D64" s="4" t="s">
         <v>240</v>
@@ -4072,7 +4062,7 @@
         <v>243</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="D65" s="4" t="s">
         <v>244</v>
@@ -4083,64 +4073,64 @@
     </row>
     <row r="66" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="4" t="s">
+        <v>242</v>
+      </c>
+      <c r="B66" s="4" t="s">
         <v>246</v>
       </c>
-      <c r="B66" s="4" t="s">
+      <c r="C66" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D66" s="4" t="s">
         <v>247</v>
       </c>
-      <c r="C66" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D66" s="4" t="s">
+      <c r="E66" s="5" t="s">
         <v>248</v>
-      </c>
-      <c r="E66" s="5" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="67" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="4" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C67" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D67" s="4" t="s">
+        <v>250</v>
+      </c>
+      <c r="E67" s="5" t="s">
         <v>251</v>
-      </c>
-      <c r="E67" s="5" t="s">
-        <v>252</v>
       </c>
     </row>
     <row r="68" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="4" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="B68" s="4" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C68" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D68" s="4" t="s">
+        <v>253</v>
+      </c>
+      <c r="E68" s="5" t="s">
         <v>254</v>
-      </c>
-      <c r="E68" s="5" t="s">
-        <v>255</v>
       </c>
     </row>
     <row r="69" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="4" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="B69" s="4" t="s">
+        <v>255</v>
+      </c>
+      <c r="C69" s="4" t="s">
         <v>256</v>
-      </c>
-      <c r="C69" s="4" t="s">
-        <v>6</v>
       </c>
       <c r="D69" s="4" t="s">
         <v>257</v>
@@ -4151,47 +4141,47 @@
     </row>
     <row r="70" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="4" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="B70" s="4" t="s">
         <v>259</v>
       </c>
       <c r="C70" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D70" s="4" t="s">
         <v>260</v>
       </c>
-      <c r="D70" s="4" t="s">
+      <c r="E70" s="5" t="s">
         <v>261</v>
-      </c>
-      <c r="E70" s="5" t="s">
-        <v>262</v>
       </c>
     </row>
     <row r="71" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="4" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C71" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D71" s="4" t="s">
+        <v>263</v>
+      </c>
+      <c r="E71" s="5" t="s">
         <v>264</v>
-      </c>
-      <c r="E71" s="5" t="s">
-        <v>265</v>
       </c>
     </row>
     <row r="72" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="4" t="s">
-        <v>246</v>
+        <v>265</v>
       </c>
       <c r="B72" s="4" t="s">
         <v>266</v>
       </c>
       <c r="C72" s="4" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="D72" s="4" t="s">
         <v>267</v>
@@ -4202,81 +4192,81 @@
     </row>
     <row r="73" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="4" t="s">
+        <v>265</v>
+      </c>
+      <c r="B73" s="4" t="s">
         <v>269</v>
       </c>
-      <c r="B73" s="4" t="s">
+      <c r="C73" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D73" s="4" t="s">
         <v>270</v>
       </c>
-      <c r="C73" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D73" s="4" t="s">
+      <c r="E73" s="5" t="s">
         <v>271</v>
-      </c>
-      <c r="E73" s="5" t="s">
-        <v>272</v>
       </c>
     </row>
     <row r="74" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="4" t="s">
-        <v>269</v>
+        <v>272</v>
       </c>
       <c r="B74" s="4" t="s">
         <v>273</v>
       </c>
       <c r="C74" s="4" t="s">
-        <v>6</v>
+        <v>274</v>
       </c>
       <c r="D74" s="4" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="E74" s="5" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
     </row>
     <row r="75" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="4" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="B75" s="4" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="C75" s="4" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="D75" s="4" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="E75" s="5" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
     </row>
     <row r="76" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="4" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="B76" s="4" t="s">
+        <v>282</v>
+      </c>
+      <c r="C76" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="D76" s="4" t="s">
         <v>283</v>
       </c>
-      <c r="C76" s="4" t="s">
-        <v>278</v>
-      </c>
-      <c r="D76" s="4" t="s">
+      <c r="E76" s="5" t="s">
         <v>284</v>
-      </c>
-      <c r="E76" s="5" t="s">
-        <v>285</v>
       </c>
     </row>
     <row r="77" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="4" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="B77" s="4" t="s">
         <v>286</v>
       </c>
       <c r="C77" s="4" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="D77" s="4" t="s">
         <v>287</v>
@@ -4287,268 +4277,268 @@
     </row>
     <row r="78" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="4" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="B78" s="4" t="s">
         <v>290</v>
       </c>
       <c r="C78" s="4" t="s">
-        <v>278</v>
+        <v>291</v>
       </c>
       <c r="D78" s="4" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="E78" s="5" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
     </row>
     <row r="79" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="4" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="B79" s="4" t="s">
         <v>294</v>
       </c>
       <c r="C79" s="4" t="s">
+        <v>291</v>
+      </c>
+      <c r="D79" s="4" t="s">
         <v>295</v>
       </c>
-      <c r="D79" s="4" t="s">
+      <c r="E79" s="5" t="s">
         <v>296</v>
-      </c>
-      <c r="E79" s="5" t="s">
-        <v>297</v>
       </c>
     </row>
     <row r="80" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="4" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="B80" s="4" t="s">
+        <v>297</v>
+      </c>
+      <c r="C80" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="D80" s="4" t="s">
         <v>298</v>
       </c>
-      <c r="C80" s="4" t="s">
-        <v>295</v>
-      </c>
-      <c r="D80" s="4" t="s">
+      <c r="E80" s="5" t="s">
         <v>299</v>
-      </c>
-      <c r="E80" s="5" t="s">
-        <v>300</v>
       </c>
     </row>
     <row r="81" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="4" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="B81" s="4" t="s">
+        <v>300</v>
+      </c>
+      <c r="C81" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="D81" s="4" t="s">
         <v>301</v>
       </c>
-      <c r="C81" s="4" t="s">
-        <v>278</v>
-      </c>
-      <c r="D81" s="4" t="s">
+      <c r="E81" s="5" t="s">
         <v>302</v>
-      </c>
-      <c r="E81" s="5" t="s">
-        <v>303</v>
       </c>
     </row>
     <row r="82" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="4" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="B82" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="C82" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="D82" s="4" t="s">
         <v>304</v>
       </c>
-      <c r="C82" s="4" t="s">
-        <v>278</v>
-      </c>
-      <c r="D82" s="4" t="s">
+      <c r="E82" s="5" t="s">
         <v>305</v>
-      </c>
-      <c r="E82" s="5" t="s">
-        <v>306</v>
       </c>
     </row>
     <row r="83" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="4" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="B83" s="4" t="s">
+        <v>306</v>
+      </c>
+      <c r="C83" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="D83" s="4" t="s">
         <v>307</v>
       </c>
-      <c r="C83" s="4" t="s">
-        <v>278</v>
-      </c>
-      <c r="D83" s="4" t="s">
+      <c r="E83" s="5" t="s">
         <v>308</v>
-      </c>
-      <c r="E83" s="5" t="s">
-        <v>309</v>
       </c>
     </row>
     <row r="84" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="4" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="B84" s="4" t="s">
+        <v>309</v>
+      </c>
+      <c r="C84" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="D84" s="4" t="s">
         <v>310</v>
       </c>
-      <c r="C84" s="4" t="s">
-        <v>278</v>
-      </c>
-      <c r="D84" s="4" t="s">
+      <c r="E84" s="5" t="s">
         <v>311</v>
-      </c>
-      <c r="E84" s="5" t="s">
-        <v>312</v>
       </c>
     </row>
     <row r="85" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="4" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="B85" s="4" t="s">
+        <v>312</v>
+      </c>
+      <c r="C85" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="D85" s="4" t="s">
         <v>313</v>
       </c>
-      <c r="C85" s="4" t="s">
-        <v>278</v>
-      </c>
-      <c r="D85" s="4" t="s">
+      <c r="E85" s="5" t="s">
         <v>314</v>
-      </c>
-      <c r="E85" s="5" t="s">
-        <v>315</v>
       </c>
     </row>
     <row r="86" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="4" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="B86" s="4" t="s">
+        <v>315</v>
+      </c>
+      <c r="C86" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="D86" s="4" t="s">
         <v>316</v>
       </c>
-      <c r="C86" s="4" t="s">
-        <v>278</v>
-      </c>
-      <c r="D86" s="4" t="s">
+      <c r="E86" s="5" t="s">
         <v>317</v>
-      </c>
-      <c r="E86" s="5" t="s">
-        <v>318</v>
       </c>
     </row>
     <row r="87" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="4" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="B87" s="4" t="s">
+        <v>318</v>
+      </c>
+      <c r="C87" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="D87" s="4" t="s">
         <v>319</v>
       </c>
-      <c r="C87" s="4" t="s">
-        <v>278</v>
-      </c>
-      <c r="D87" s="4" t="s">
+      <c r="E87" s="5" t="s">
         <v>320</v>
-      </c>
-      <c r="E87" s="5" t="s">
-        <v>321</v>
       </c>
     </row>
     <row r="88" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="4" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="B88" s="4" t="s">
+        <v>321</v>
+      </c>
+      <c r="C88" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="D88" s="4" t="s">
         <v>322</v>
       </c>
-      <c r="C88" s="4" t="s">
-        <v>278</v>
-      </c>
-      <c r="D88" s="4" t="s">
+      <c r="E88" s="5" t="s">
         <v>323</v>
-      </c>
-      <c r="E88" s="5" t="s">
-        <v>324</v>
       </c>
     </row>
     <row r="89" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="4" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="B89" s="4" t="s">
+        <v>324</v>
+      </c>
+      <c r="C89" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="D89" s="4" t="s">
         <v>325</v>
       </c>
-      <c r="C89" s="4" t="s">
-        <v>278</v>
-      </c>
-      <c r="D89" s="4" t="s">
+      <c r="E89" s="5" t="s">
         <v>326</v>
-      </c>
-      <c r="E89" s="5" t="s">
-        <v>327</v>
       </c>
     </row>
     <row r="90" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="4" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="B90" s="4" t="s">
+        <v>327</v>
+      </c>
+      <c r="C90" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="D90" s="4" t="s">
         <v>328</v>
       </c>
-      <c r="C90" s="4" t="s">
-        <v>278</v>
-      </c>
-      <c r="D90" s="4" t="s">
+      <c r="E90" s="5" t="s">
         <v>329</v>
-      </c>
-      <c r="E90" s="5" t="s">
-        <v>330</v>
       </c>
     </row>
     <row r="91" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="4" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="B91" s="4" t="s">
+        <v>330</v>
+      </c>
+      <c r="C91" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="D91" s="4" t="s">
         <v>331</v>
       </c>
-      <c r="C91" s="4" t="s">
-        <v>278</v>
-      </c>
-      <c r="D91" s="4" t="s">
+      <c r="E91" s="5" t="s">
         <v>332</v>
-      </c>
-      <c r="E91" s="5" t="s">
-        <v>333</v>
       </c>
     </row>
     <row r="92" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="4" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="B92" s="4" t="s">
+        <v>333</v>
+      </c>
+      <c r="C92" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="D92" s="4" t="s">
         <v>334</v>
       </c>
-      <c r="C92" s="4" t="s">
-        <v>278</v>
-      </c>
-      <c r="D92" s="4" t="s">
+      <c r="E92" s="5" t="s">
         <v>335</v>
-      </c>
-      <c r="E92" s="5" t="s">
-        <v>336</v>
       </c>
     </row>
     <row r="93" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="4" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="B93" s="4" t="s">
+        <v>336</v>
+      </c>
+      <c r="C93" s="4" t="s">
         <v>337</v>
-      </c>
-      <c r="C93" s="4" t="s">
-        <v>278</v>
       </c>
       <c r="D93" s="4" t="s">
         <v>338</v>
@@ -4559,30 +4549,30 @@
     </row>
     <row r="94" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="4" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="B94" s="4" t="s">
         <v>340</v>
       </c>
       <c r="C94" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="D94" s="4" t="s">
         <v>341</v>
       </c>
-      <c r="D94" s="4" t="s">
+      <c r="E94" s="5" t="s">
         <v>342</v>
-      </c>
-      <c r="E94" s="5" t="s">
-        <v>343</v>
       </c>
     </row>
     <row r="95" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="4" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="B95" s="4" t="s">
+        <v>343</v>
+      </c>
+      <c r="C95" s="4" t="s">
         <v>344</v>
-      </c>
-      <c r="C95" s="4" t="s">
-        <v>278</v>
       </c>
       <c r="D95" s="4" t="s">
         <v>345</v>
@@ -4593,254 +4583,254 @@
     </row>
     <row r="96" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="4" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="B96" s="4" t="s">
         <v>347</v>
       </c>
       <c r="C96" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="D96" s="4" t="s">
         <v>348</v>
       </c>
-      <c r="D96" s="4" t="s">
+      <c r="E96" s="5" t="s">
         <v>349</v>
-      </c>
-      <c r="E96" s="5" t="s">
-        <v>350</v>
       </c>
     </row>
     <row r="97" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="4" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="B97" s="4" t="s">
+        <v>350</v>
+      </c>
+      <c r="C97" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="D97" s="4" t="s">
         <v>351</v>
       </c>
-      <c r="C97" s="4" t="s">
-        <v>278</v>
-      </c>
-      <c r="D97" s="4" t="s">
+      <c r="E97" s="5" t="s">
         <v>352</v>
-      </c>
-      <c r="E97" s="5" t="s">
-        <v>353</v>
       </c>
     </row>
     <row r="98" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="4" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="B98" s="4" t="s">
+        <v>353</v>
+      </c>
+      <c r="C98" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="D98" s="4" t="s">
         <v>354</v>
       </c>
-      <c r="C98" s="4" t="s">
-        <v>278</v>
-      </c>
-      <c r="D98" s="4" t="s">
+      <c r="E98" s="5" t="s">
         <v>355</v>
-      </c>
-      <c r="E98" s="5" t="s">
-        <v>356</v>
       </c>
     </row>
     <row r="99" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="4" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="B99" s="4" t="s">
-        <v>357</v>
+        <v>359</v>
       </c>
       <c r="C99" s="4" t="s">
-        <v>278</v>
+        <v>360</v>
       </c>
       <c r="D99" s="4" t="s">
-        <v>358</v>
+        <v>361</v>
       </c>
       <c r="E99" s="5" t="s">
-        <v>359</v>
+        <v>362</v>
       </c>
     </row>
     <row r="100" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="4" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="B100" s="4" t="s">
         <v>363</v>
       </c>
       <c r="C100" s="4" t="s">
+        <v>291</v>
+      </c>
+      <c r="D100" s="4" t="s">
         <v>364</v>
       </c>
-      <c r="D100" s="4" t="s">
+      <c r="E100" s="5" t="s">
         <v>365</v>
-      </c>
-      <c r="E100" s="5" t="s">
-        <v>366</v>
       </c>
     </row>
     <row r="101" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="4" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="B101" s="4" t="s">
+        <v>366</v>
+      </c>
+      <c r="C101" s="4" t="s">
+        <v>291</v>
+      </c>
+      <c r="D101" s="4" t="s">
         <v>367</v>
       </c>
-      <c r="C101" s="4" t="s">
-        <v>295</v>
-      </c>
-      <c r="D101" s="4" t="s">
+      <c r="E101" s="5" t="s">
         <v>368</v>
-      </c>
-      <c r="E101" s="5" t="s">
-        <v>369</v>
       </c>
     </row>
     <row r="102" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="4" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="B102" s="4" t="s">
+        <v>369</v>
+      </c>
+      <c r="C102" s="4" t="s">
+        <v>291</v>
+      </c>
+      <c r="D102" s="4" t="s">
         <v>370</v>
       </c>
-      <c r="C102" s="4" t="s">
-        <v>295</v>
-      </c>
-      <c r="D102" s="4" t="s">
+      <c r="E102" s="5" t="s">
         <v>371</v>
-      </c>
-      <c r="E102" s="5" t="s">
-        <v>372</v>
       </c>
     </row>
     <row r="103" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="4" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="B103" s="4" t="s">
+        <v>372</v>
+      </c>
+      <c r="C103" s="4" t="s">
+        <v>291</v>
+      </c>
+      <c r="D103" s="4" t="s">
         <v>373</v>
       </c>
-      <c r="C103" s="4" t="s">
-        <v>295</v>
-      </c>
-      <c r="D103" s="4" t="s">
+      <c r="E103" s="5" t="s">
         <v>374</v>
-      </c>
-      <c r="E103" s="5" t="s">
-        <v>375</v>
       </c>
     </row>
     <row r="104" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="4" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="B104" s="4" t="s">
+        <v>375</v>
+      </c>
+      <c r="C104" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="D104" s="4" t="s">
         <v>376</v>
       </c>
-      <c r="C104" s="4" t="s">
-        <v>295</v>
-      </c>
-      <c r="D104" s="4" t="s">
+      <c r="E104" s="5" t="s">
         <v>377</v>
-      </c>
-      <c r="E104" s="5" t="s">
-        <v>378</v>
       </c>
     </row>
     <row r="105" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" s="4" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="B105" s="4" t="s">
+        <v>378</v>
+      </c>
+      <c r="C105" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="D105" s="4" t="s">
         <v>379</v>
       </c>
-      <c r="C105" s="4" t="s">
-        <v>278</v>
-      </c>
-      <c r="D105" s="4" t="s">
+      <c r="E105" s="5" t="s">
         <v>380</v>
-      </c>
-      <c r="E105" s="5" t="s">
-        <v>381</v>
       </c>
     </row>
     <row r="106" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="4" t="s">
-        <v>276</v>
+        <v>381</v>
       </c>
       <c r="B106" s="4" t="s">
+        <v>315</v>
+      </c>
+      <c r="C106" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="D106" s="4" t="s">
         <v>382</v>
       </c>
-      <c r="C106" s="4" t="s">
-        <v>278</v>
-      </c>
-      <c r="D106" s="4" t="s">
+      <c r="E106" s="5" t="s">
         <v>383</v>
-      </c>
-      <c r="E106" s="5" t="s">
-        <v>384</v>
       </c>
     </row>
     <row r="107" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" s="4" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
       <c r="B107" s="4" t="s">
-        <v>319</v>
+        <v>333</v>
       </c>
       <c r="C107" s="4" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="D107" s="4" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="E107" s="5" t="s">
-        <v>387</v>
+        <v>335</v>
       </c>
     </row>
     <row r="108" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" s="4" t="s">
+        <v>381</v>
+      </c>
+      <c r="B108" s="4" t="s">
+        <v>336</v>
+      </c>
+      <c r="C108" s="4" t="s">
         <v>385</v>
       </c>
-      <c r="B108" s="4" t="s">
-        <v>337</v>
-      </c>
-      <c r="C108" s="4" t="s">
-        <v>278</v>
-      </c>
       <c r="D108" s="4" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="E108" s="5" t="s">
-        <v>339</v>
+        <v>387</v>
       </c>
     </row>
     <row r="109" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" s="4" t="s">
-        <v>385</v>
+        <v>388</v>
       </c>
       <c r="B109" s="4" t="s">
-        <v>340</v>
+        <v>315</v>
       </c>
       <c r="C109" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="D109" s="4" t="s">
         <v>389</v>
       </c>
-      <c r="D109" s="4" t="s">
-        <v>390</v>
-      </c>
       <c r="E109" s="5" t="s">
-        <v>391</v>
+        <v>383</v>
       </c>
     </row>
     <row r="110" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" s="4" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
       <c r="B110" s="4" t="s">
-        <v>319</v>
+        <v>336</v>
       </c>
       <c r="C110" s="4" t="s">
-        <v>278</v>
+        <v>337</v>
       </c>
       <c r="D110" s="4" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="E110" s="5" t="s">
         <v>387</v>
@@ -4848,19 +4838,19 @@
     </row>
     <row r="111" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" s="4" t="s">
-        <v>392</v>
+        <v>395</v>
       </c>
       <c r="B111" s="4" t="s">
-        <v>340</v>
+        <v>369</v>
       </c>
       <c r="C111" s="4" t="s">
-        <v>341</v>
+        <v>291</v>
       </c>
       <c r="D111" s="4" t="s">
-        <v>395</v>
+        <v>398</v>
       </c>
       <c r="E111" s="5" t="s">
-        <v>391</v>
+        <v>371</v>
       </c>
     </row>
     <row r="112" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -4868,591 +4858,591 @@
         <v>399</v>
       </c>
       <c r="B112" s="4" t="s">
-        <v>373</v>
+        <v>336</v>
       </c>
       <c r="C112" s="4" t="s">
-        <v>295</v>
+        <v>337</v>
       </c>
       <c r="D112" s="4" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="E112" s="5" t="s">
-        <v>375</v>
+        <v>396</v>
       </c>
     </row>
     <row r="113" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" s="4" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="B113" s="4" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="C113" s="4" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="D113" s="4" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="E113" s="5" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
     </row>
     <row r="114" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114" s="4" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="B114" s="4" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="C114" s="4" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="D114" s="4" t="s">
-        <v>406</v>
+        <v>411</v>
       </c>
       <c r="E114" s="5" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
     </row>
     <row r="115" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" s="4" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
       <c r="B115" s="4" t="s">
-        <v>340</v>
+        <v>369</v>
       </c>
       <c r="C115" s="4" t="s">
-        <v>341</v>
+        <v>291</v>
       </c>
       <c r="D115" s="4" t="s">
-        <v>415</v>
+        <v>417</v>
       </c>
       <c r="E115" s="5" t="s">
-        <v>400</v>
+        <v>371</v>
       </c>
     </row>
     <row r="116" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116" s="4" t="s">
-        <v>407</v>
+        <v>419</v>
       </c>
       <c r="B116" s="4" t="s">
-        <v>373</v>
+        <v>336</v>
       </c>
       <c r="C116" s="4" t="s">
-        <v>295</v>
+        <v>337</v>
       </c>
       <c r="D116" s="4" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="E116" s="5" t="s">
-        <v>375</v>
+        <v>396</v>
       </c>
     </row>
     <row r="117" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A117" s="4" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="B117" s="4" t="s">
-        <v>340</v>
+        <v>273</v>
       </c>
       <c r="C117" s="4" t="s">
-        <v>341</v>
+        <v>274</v>
       </c>
       <c r="D117" s="4" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="E117" s="5" t="s">
-        <v>400</v>
+        <v>276</v>
       </c>
     </row>
     <row r="118" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118" s="4" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="B118" s="4" t="s">
         <v>277</v>
       </c>
       <c r="C118" s="4" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="D118" s="4" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="E118" s="5" t="s">
-        <v>280</v>
+        <v>404</v>
       </c>
     </row>
     <row r="119" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A119" s="4" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="B119" s="4" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="C119" s="4" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="D119" s="4" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
       <c r="E119" s="5" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
     </row>
     <row r="120" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A120" s="4" t="s">
+        <v>421</v>
+      </c>
+      <c r="B120" s="4" t="s">
+        <v>279</v>
+      </c>
+      <c r="C120" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="D120" s="4" t="s">
         <v>425</v>
       </c>
-      <c r="B120" s="4" t="s">
-        <v>282</v>
-      </c>
-      <c r="C120" s="4" t="s">
-        <v>278</v>
-      </c>
-      <c r="D120" s="4" t="s">
-        <v>428</v>
-      </c>
       <c r="E120" s="5" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
     </row>
     <row r="121" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A121" s="4" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="B121" s="4" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C121" s="4" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="D121" s="4" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
       <c r="E121" s="5" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
     </row>
     <row r="122" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A122" s="4" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="B122" s="4" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C122" s="4" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="D122" s="4" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="E122" s="5" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
     </row>
     <row r="123" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A123" s="4" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="B123" s="4" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="C123" s="4" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="D123" s="4" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
       <c r="E123" s="5" t="s">
-        <v>412</v>
+        <v>288</v>
       </c>
     </row>
     <row r="124" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A124" s="4" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="B124" s="4" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C124" s="4" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="D124" s="4" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="E124" s="5" t="s">
-        <v>292</v>
+        <v>409</v>
       </c>
     </row>
     <row r="125" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A125" s="4" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="B125" s="4" t="s">
+        <v>290</v>
+      </c>
+      <c r="C125" s="4" t="s">
+        <v>291</v>
+      </c>
+      <c r="D125" s="4" t="s">
+        <v>430</v>
+      </c>
+      <c r="E125" s="5" t="s">
         <v>293</v>
-      </c>
-      <c r="C125" s="4" t="s">
-        <v>278</v>
-      </c>
-      <c r="D125" s="4" t="s">
-        <v>433</v>
-      </c>
-      <c r="E125" s="5" t="s">
-        <v>413</v>
       </c>
     </row>
     <row r="126" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A126" s="4" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="B126" s="4" t="s">
         <v>294</v>
       </c>
       <c r="C126" s="4" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="D126" s="4" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="E126" s="5" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="127" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A127" s="4" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="B127" s="4" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C127" s="4" t="s">
-        <v>295</v>
+        <v>274</v>
       </c>
       <c r="D127" s="4" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="E127" s="5" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="128" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A128" s="4" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="B128" s="4" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C128" s="4" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="D128" s="4" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="E128" s="5" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="129" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A129" s="4" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="B129" s="4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C129" s="4" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="D129" s="4" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="E129" s="5" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="130" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A130" s="4" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="B130" s="4" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C130" s="4" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="D130" s="4" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="E130" s="5" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="131" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A131" s="4" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="B131" s="4" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C131" s="4" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="D131" s="4" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="E131" s="5" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="132" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A132" s="4" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="B132" s="4" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C132" s="4" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="D132" s="4" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
       <c r="E132" s="5" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="133" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A133" s="4" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="B133" s="4" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C133" s="4" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="D133" s="4" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="E133" s="5" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="134" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A134" s="4" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="B134" s="4" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C134" s="4" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="D134" s="4" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
       <c r="E134" s="5" t="s">
-        <v>321</v>
+        <v>410</v>
       </c>
     </row>
     <row r="135" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A135" s="4" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="B135" s="4" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C135" s="4" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="D135" s="4" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="E135" s="5" t="s">
-        <v>414</v>
+        <v>323</v>
       </c>
     </row>
     <row r="136" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A136" s="4" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="B136" s="4" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C136" s="4" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="D136" s="4" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="E136" s="5" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="137" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A137" s="4" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="B137" s="4" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="C137" s="4" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="D137" s="4" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="E137" s="5" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="138" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A138" s="4" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="B138" s="4" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C138" s="4" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="D138" s="4" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
       <c r="E138" s="5" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="139" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A139" s="4" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="B139" s="4" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C139" s="4" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="D139" s="4" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
       <c r="E139" s="5" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="140" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A140" s="4" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="B140" s="4" t="s">
+        <v>336</v>
+      </c>
+      <c r="C140" s="4" t="s">
         <v>337</v>
       </c>
-      <c r="C140" s="4" t="s">
-        <v>278</v>
-      </c>
       <c r="D140" s="4" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
       <c r="E140" s="5" t="s">
-        <v>339</v>
+        <v>396</v>
       </c>
     </row>
     <row r="141" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A141" s="4" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="B141" s="4" t="s">
         <v>340</v>
       </c>
       <c r="C141" s="4" t="s">
-        <v>341</v>
+        <v>274</v>
       </c>
       <c r="D141" s="4" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="E141" s="5" t="s">
-        <v>400</v>
+        <v>412</v>
       </c>
     </row>
     <row r="142" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A142" s="4" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="B142" s="4" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C142" s="4" t="s">
-        <v>278</v>
+        <v>447</v>
       </c>
       <c r="D142" s="4" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="E142" s="5" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
     </row>
     <row r="143" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A143" s="4" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="B143" s="4" t="s">
         <v>347</v>
       </c>
       <c r="C143" s="4" t="s">
-        <v>451</v>
+        <v>274</v>
       </c>
       <c r="D143" s="4" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
       <c r="E143" s="5" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
     </row>
     <row r="144" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A144" s="4" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="B144" s="4" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="C144" s="4" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="D144" s="4" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="E144" s="5" t="s">
-        <v>418</v>
+        <v>392</v>
       </c>
     </row>
     <row r="145" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A145" s="4" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="B145" s="4" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="C145" s="4" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="D145" s="4" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
       <c r="E145" s="5" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
     </row>
     <row r="146" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A146" s="4" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="B146" s="4" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="C146" s="4" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="D146" s="4" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
       <c r="E146" s="5" t="s">
         <v>397</v>
@@ -5460,234 +5450,234 @@
     </row>
     <row r="147" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A147" s="4" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="B147" s="4" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="C147" s="4" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="D147" s="4" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="E147" s="5" t="s">
-        <v>401</v>
+        <v>415</v>
       </c>
     </row>
     <row r="148" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A148" s="4" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="B148" s="4" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="C148" s="4" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="D148" s="4" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
       <c r="E148" s="5" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
     </row>
     <row r="149" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A149" s="4" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="B149" s="4" t="s">
+        <v>359</v>
+      </c>
+      <c r="C149" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="D149" s="4" t="s">
+        <v>455</v>
+      </c>
+      <c r="E149" s="5" t="s">
         <v>362</v>
-      </c>
-      <c r="C149" s="4" t="s">
-        <v>278</v>
-      </c>
-      <c r="D149" s="4" t="s">
-        <v>458</v>
-      </c>
-      <c r="E149" s="5" t="s">
-        <v>420</v>
       </c>
     </row>
     <row r="150" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A150" s="4" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="B150" s="4" t="s">
         <v>363</v>
       </c>
       <c r="C150" s="4" t="s">
-        <v>278</v>
+        <v>291</v>
       </c>
       <c r="D150" s="4" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
       <c r="E150" s="5" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="151" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A151" s="4" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="B151" s="4" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="C151" s="4" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="D151" s="4" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
       <c r="E151" s="5" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="152" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A152" s="4" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="B152" s="4" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="C152" s="4" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="D152" s="4" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
       <c r="E152" s="5" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="153" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A153" s="4" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="B153" s="4" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="C153" s="4" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="D153" s="4" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
       <c r="E153" s="5" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="154" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A154" s="4" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="B154" s="4" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="C154" s="4" t="s">
-        <v>295</v>
+        <v>274</v>
       </c>
       <c r="D154" s="4" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="E154" s="5" t="s">
-        <v>378</v>
+        <v>418</v>
       </c>
     </row>
     <row r="155" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A155" s="4" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="B155" s="4" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C155" s="4" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="D155" s="4" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
       <c r="E155" s="5" t="s">
-        <v>422</v>
+        <v>394</v>
       </c>
     </row>
     <row r="156" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A156" s="4" t="s">
-        <v>425</v>
+        <v>462</v>
       </c>
       <c r="B156" s="4" t="s">
-        <v>382</v>
+        <v>315</v>
       </c>
       <c r="C156" s="4" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="D156" s="4" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="E156" s="5" t="s">
-        <v>398</v>
+        <v>383</v>
       </c>
     </row>
     <row r="157" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A157" s="4" t="s">
-        <v>466</v>
+        <v>462</v>
       </c>
       <c r="B157" s="4" t="s">
-        <v>319</v>
+        <v>333</v>
       </c>
       <c r="C157" s="4" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="D157" s="4" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="E157" s="5" t="s">
-        <v>387</v>
+        <v>390</v>
       </c>
     </row>
     <row r="158" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A158" s="4" t="s">
+        <v>462</v>
+      </c>
+      <c r="B158" s="4" t="s">
+        <v>336</v>
+      </c>
+      <c r="C158" s="4" t="s">
+        <v>385</v>
+      </c>
+      <c r="D158" s="4" t="s">
+        <v>465</v>
+      </c>
+      <c r="E158" s="5" t="s">
         <v>466</v>
-      </c>
-      <c r="B158" s="4" t="s">
-        <v>337</v>
-      </c>
-      <c r="C158" s="4" t="s">
-        <v>278</v>
-      </c>
-      <c r="D158" s="4" t="s">
-        <v>468</v>
-      </c>
-      <c r="E158" s="5" t="s">
-        <v>394</v>
       </c>
     </row>
     <row r="159" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A159" s="4" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="B159" s="4" t="s">
-        <v>340</v>
+        <v>468</v>
       </c>
       <c r="C159" s="4" t="s">
-        <v>389</v>
+        <v>469</v>
       </c>
       <c r="D159" s="4" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="E159" s="5" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
     </row>
     <row r="160" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A160" s="4" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="B160" s="4" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="C160" s="4" t="s">
-        <v>473</v>
+        <v>6</v>
       </c>
       <c r="D160" s="4" t="s">
         <v>474</v>
@@ -5698,36 +5688,36 @@
     </row>
     <row r="161" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A161" s="4" t="s">
+        <v>472</v>
+      </c>
+      <c r="B161" s="4" t="s">
         <v>476</v>
       </c>
-      <c r="B161" s="4" t="s">
+      <c r="C161" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D161" s="4" t="s">
         <v>477</v>
       </c>
-      <c r="C161" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D161" s="4" t="s">
+      <c r="E161" s="5" t="s">
         <v>478</v>
-      </c>
-      <c r="E161" s="5" t="s">
-        <v>479</v>
       </c>
     </row>
     <row r="162" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A162" s="4" t="s">
-        <v>476</v>
+        <v>480</v>
       </c>
       <c r="B162" s="4" t="s">
-        <v>480</v>
-      </c>
-      <c r="C162" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D162" s="4" t="s">
+        <v>479</v>
+      </c>
+      <c r="C162" s="5" t="s">
         <v>481</v>
       </c>
+      <c r="D162" s="5" t="s">
+        <v>482</v>
+      </c>
       <c r="E162" s="5" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
     </row>
     <row r="163" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -5735,131 +5725,131 @@
         <v>484</v>
       </c>
       <c r="B163" s="4" t="s">
-        <v>483</v>
+        <v>479</v>
       </c>
       <c r="C163" s="5" t="s">
+        <v>481</v>
+      </c>
+      <c r="D163" s="5" t="s">
         <v>485</v>
       </c>
-      <c r="D163" s="5" t="s">
+      <c r="E163" s="5" t="s">
         <v>486</v>
-      </c>
-      <c r="E163" s="5" t="s">
-        <v>487</v>
       </c>
     </row>
     <row r="164" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A164" s="4" t="s">
+        <v>487</v>
+      </c>
+      <c r="B164" s="4" t="s">
+        <v>479</v>
+      </c>
+      <c r="C164" s="5" t="s">
+        <v>481</v>
+      </c>
+      <c r="D164" s="5" t="s">
         <v>488</v>
       </c>
-      <c r="B164" s="4" t="s">
-        <v>483</v>
-      </c>
-      <c r="C164" s="5" t="s">
-        <v>485</v>
-      </c>
-      <c r="D164" s="5" t="s">
+      <c r="E164" s="5" t="s">
         <v>489</v>
-      </c>
-      <c r="E164" s="5" t="s">
-        <v>490</v>
       </c>
     </row>
     <row r="165" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A165" s="4" t="s">
+        <v>490</v>
+      </c>
+      <c r="B165" s="4" t="s">
+        <v>479</v>
+      </c>
+      <c r="C165" s="5" t="s">
+        <v>481</v>
+      </c>
+      <c r="D165" s="5" t="s">
         <v>491</v>
       </c>
-      <c r="B165" s="4" t="s">
-        <v>483</v>
-      </c>
-      <c r="C165" s="5" t="s">
-        <v>485</v>
-      </c>
-      <c r="D165" s="5" t="s">
+      <c r="E165" s="5" t="s">
         <v>492</v>
-      </c>
-      <c r="E165" s="5" t="s">
-        <v>493</v>
       </c>
     </row>
     <row r="166" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A166" s="4" t="s">
+        <v>493</v>
+      </c>
+      <c r="B166" s="4" t="s">
+        <v>479</v>
+      </c>
+      <c r="C166" s="5" t="s">
+        <v>481</v>
+      </c>
+      <c r="D166" s="5" t="s">
         <v>494</v>
       </c>
-      <c r="B166" s="4" t="s">
-        <v>483</v>
-      </c>
-      <c r="C166" s="5" t="s">
-        <v>485</v>
-      </c>
-      <c r="D166" s="5" t="s">
+      <c r="E166" s="5" t="s">
         <v>495</v>
-      </c>
-      <c r="E166" s="5" t="s">
-        <v>496</v>
       </c>
     </row>
     <row r="167" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A167" s="4" t="s">
+        <v>496</v>
+      </c>
+      <c r="B167" s="4" t="s">
+        <v>479</v>
+      </c>
+      <c r="C167" s="5" t="s">
+        <v>481</v>
+      </c>
+      <c r="D167" s="5" t="s">
         <v>497</v>
       </c>
-      <c r="B167" s="4" t="s">
-        <v>483</v>
-      </c>
-      <c r="C167" s="5" t="s">
-        <v>485</v>
-      </c>
-      <c r="D167" s="5" t="s">
+      <c r="E167" s="5" t="s">
         <v>498</v>
-      </c>
-      <c r="E167" s="5" t="s">
-        <v>499</v>
       </c>
     </row>
     <row r="168" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A168" s="4" t="s">
+        <v>499</v>
+      </c>
+      <c r="B168" s="4" t="s">
+        <v>479</v>
+      </c>
+      <c r="C168" s="5" t="s">
+        <v>481</v>
+      </c>
+      <c r="D168" s="5" t="s">
         <v>500</v>
       </c>
-      <c r="B168" s="4" t="s">
-        <v>483</v>
-      </c>
-      <c r="C168" s="5" t="s">
-        <v>485</v>
-      </c>
-      <c r="D168" s="5" t="s">
+      <c r="E168" s="5" t="s">
         <v>501</v>
-      </c>
-      <c r="E168" s="5" t="s">
-        <v>502</v>
       </c>
     </row>
     <row r="169" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A169" s="4" t="s">
+        <v>502</v>
+      </c>
+      <c r="B169" s="4" t="s">
+        <v>479</v>
+      </c>
+      <c r="C169" s="5" t="s">
+        <v>481</v>
+      </c>
+      <c r="D169" s="5" t="s">
         <v>503</v>
       </c>
-      <c r="B169" s="4" t="s">
-        <v>483</v>
-      </c>
-      <c r="C169" s="5" t="s">
-        <v>485</v>
-      </c>
-      <c r="D169" s="5" t="s">
+      <c r="E169" s="5" t="s">
         <v>504</v>
-      </c>
-      <c r="E169" s="5" t="s">
-        <v>505</v>
       </c>
     </row>
     <row r="170" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A170" s="4" t="s">
+        <v>505</v>
+      </c>
+      <c r="B170" s="4" t="s">
         <v>506</v>
       </c>
-      <c r="B170" s="4" t="s">
-        <v>483</v>
-      </c>
-      <c r="C170" s="5" t="s">
-        <v>485</v>
-      </c>
-      <c r="D170" s="5" t="s">
+      <c r="C170" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D170" s="4" t="s">
         <v>507</v>
       </c>
       <c r="E170" s="5" t="s">
@@ -5868,75 +5858,75 @@
     </row>
     <row r="171" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A171" s="4" t="s">
+        <v>505</v>
+      </c>
+      <c r="B171" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="C171" s="5" t="s">
         <v>509</v>
       </c>
-      <c r="B171" s="4" t="s">
+      <c r="D171" s="4" t="s">
         <v>510</v>
       </c>
-      <c r="C171" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D171" s="4" t="s">
+      <c r="E171" s="5" t="s">
         <v>511</v>
-      </c>
-      <c r="E171" s="5" t="s">
-        <v>512</v>
       </c>
     </row>
     <row r="172" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A172" s="4" t="s">
-        <v>509</v>
+        <v>505</v>
       </c>
       <c r="B172" s="4" t="s">
-        <v>206</v>
-      </c>
-      <c r="C172" s="5" t="s">
+        <v>512</v>
+      </c>
+      <c r="C172" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D172" s="4" t="s">
         <v>513</v>
       </c>
-      <c r="D172" s="4" t="s">
+      <c r="E172" s="5" t="s">
         <v>514</v>
-      </c>
-      <c r="E172" s="5" t="s">
-        <v>515</v>
       </c>
     </row>
     <row r="173" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A173" s="4" t="s">
-        <v>509</v>
+        <v>505</v>
       </c>
       <c r="B173" s="4" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="C173" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D173" s="4" t="s">
+        <v>516</v>
+      </c>
+      <c r="E173" s="5" t="s">
         <v>517</v>
-      </c>
-      <c r="E173" s="5" t="s">
-        <v>518</v>
       </c>
     </row>
     <row r="174" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A174" s="4" t="s">
-        <v>509</v>
+        <v>505</v>
       </c>
       <c r="B174" s="4" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="C174" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D174" s="4" t="s">
+        <v>519</v>
+      </c>
+      <c r="E174" s="5" t="s">
         <v>520</v>
-      </c>
-      <c r="E174" s="5" t="s">
-        <v>521</v>
       </c>
     </row>
     <row r="175" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A175" s="4" t="s">
-        <v>509</v>
+        <v>521</v>
       </c>
       <c r="B175" s="4" t="s">
         <v>522</v>
@@ -5987,30 +5977,30 @@
     </row>
     <row r="178" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A178" s="4" t="s">
+        <v>529</v>
+      </c>
+      <c r="B178" s="4" t="s">
         <v>533</v>
-      </c>
-      <c r="B178" s="4" t="s">
-        <v>534</v>
       </c>
       <c r="C178" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D178" s="4" t="s">
+        <v>534</v>
+      </c>
+      <c r="E178" s="5" t="s">
         <v>535</v>
-      </c>
-      <c r="E178" s="5" t="s">
-        <v>536</v>
       </c>
     </row>
     <row r="179" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A179" s="4" t="s">
-        <v>533</v>
+        <v>529</v>
       </c>
       <c r="B179" s="4" t="s">
+        <v>536</v>
+      </c>
+      <c r="C179" s="4" t="s">
         <v>537</v>
-      </c>
-      <c r="C179" s="4" t="s">
-        <v>6</v>
       </c>
       <c r="D179" s="4" t="s">
         <v>538</v>
@@ -6021,13 +6011,13 @@
     </row>
     <row r="180" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A180" s="4" t="s">
-        <v>533</v>
+        <v>540</v>
       </c>
       <c r="B180" s="4" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
       <c r="C180" s="4" t="s">
-        <v>541</v>
+        <v>6</v>
       </c>
       <c r="D180" s="4" t="s">
         <v>542</v>
@@ -6044,7 +6034,7 @@
         <v>545</v>
       </c>
       <c r="C181" s="4" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="D181" s="4" t="s">
         <v>546</v>
@@ -6061,35 +6051,35 @@
         <v>549</v>
       </c>
       <c r="C182" s="4" t="s">
-        <v>25</v>
+        <v>550</v>
       </c>
       <c r="D182" s="4" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="E182" s="5" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
     </row>
     <row r="183" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A183" s="4" t="s">
-        <v>552</v>
+        <v>553</v>
       </c>
       <c r="B183" s="4" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
       <c r="C183" s="4" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
       <c r="D183" s="4" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="E183" s="5" t="s">
-        <v>556</v>
+        <v>557</v>
       </c>
     </row>
     <row r="184" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A184" s="4" t="s">
-        <v>557</v>
+        <v>553</v>
       </c>
       <c r="B184" s="4" t="s">
         <v>558</v>
@@ -6106,13 +6096,13 @@
     </row>
     <row r="185" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A185" s="4" t="s">
-        <v>557</v>
+        <v>562</v>
       </c>
       <c r="B185" s="4" t="s">
-        <v>562</v>
+        <v>563</v>
       </c>
       <c r="C185" s="4" t="s">
-        <v>563</v>
+        <v>6</v>
       </c>
       <c r="D185" s="4" t="s">
         <v>564</v>
@@ -6145,25 +6135,25 @@
       <c r="B187" s="4" t="s">
         <v>571</v>
       </c>
-      <c r="C187" s="4" t="s">
-        <v>6</v>
+      <c r="C187" s="5" t="s">
+        <v>572</v>
       </c>
       <c r="D187" s="4" t="s">
-        <v>572</v>
+        <v>573</v>
       </c>
       <c r="E187" s="5" t="s">
-        <v>573</v>
+        <v>574</v>
       </c>
     </row>
     <row r="188" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A188" s="4" t="s">
-        <v>574</v>
+        <v>575</v>
       </c>
       <c r="B188" s="4" t="s">
-        <v>575</v>
-      </c>
-      <c r="C188" s="5" t="s">
         <v>576</v>
+      </c>
+      <c r="C188" s="4" t="s">
+        <v>550</v>
       </c>
       <c r="D188" s="4" t="s">
         <v>577</v>
@@ -6173,71 +6163,71 @@
       </c>
     </row>
     <row r="189" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A189" s="4" t="s">
+      <c r="A189" s="1" t="s">
         <v>579</v>
       </c>
-      <c r="B189" s="4" t="s">
+      <c r="B189" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="C189" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="D189" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="E189" s="5" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="190" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A190" s="4" t="s">
         <v>580</v>
       </c>
-      <c r="C189" s="4" t="s">
-        <v>554</v>
-      </c>
-      <c r="D189" s="4" t="s">
+      <c r="B190" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="C190" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D190" s="4" t="s">
+        <v>510</v>
+      </c>
+      <c r="E190" s="5" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="191" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A191" s="1" t="s">
+        <v>580</v>
+      </c>
+      <c r="B191" s="1" t="s">
+        <v>515</v>
+      </c>
+      <c r="C191" s="5" t="s">
+        <v>509</v>
+      </c>
+      <c r="D191" s="4" t="s">
+        <v>516</v>
+      </c>
+      <c r="E191" s="5" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="192" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A192" s="4" t="s">
         <v>581</v>
       </c>
-      <c r="E189" s="5" t="s">
+      <c r="B192" s="4" t="s">
         <v>582</v>
       </c>
-    </row>
-    <row r="190" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A190" s="1" t="s">
+      <c r="C192" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D192" s="4" t="s">
         <v>583</v>
       </c>
-      <c r="B190" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="C190" s="5" t="s">
-        <v>207</v>
-      </c>
-      <c r="D190" s="5" t="s">
-        <v>208</v>
-      </c>
-      <c r="E190" s="5" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="191" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A191" s="4" t="s">
+      <c r="E192" s="5" t="s">
         <v>584</v>
-      </c>
-      <c r="B191" s="4" t="s">
-        <v>206</v>
-      </c>
-      <c r="C191" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D191" s="4" t="s">
-        <v>514</v>
-      </c>
-      <c r="E191" s="5" t="s">
-        <v>515</v>
-      </c>
-    </row>
-    <row r="192" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A192" s="1" t="s">
-        <v>584</v>
-      </c>
-      <c r="B192" s="1" t="s">
-        <v>519</v>
-      </c>
-      <c r="C192" s="5" t="s">
-        <v>513</v>
-      </c>
-      <c r="D192" s="4" t="s">
-        <v>520</v>
-      </c>
-      <c r="E192" s="5" t="s">
-        <v>521</v>
       </c>
     </row>
     <row r="193" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -6248,13 +6238,13 @@
         <v>586</v>
       </c>
       <c r="C193" s="4" t="s">
-        <v>25</v>
+        <v>587</v>
       </c>
       <c r="D193" s="4" t="s">
-        <v>587</v>
-      </c>
-      <c r="E193" s="5" t="s">
         <v>588</v>
+      </c>
+      <c r="E193" s="4" t="s">
+        <v>586</v>
       </c>
     </row>
     <row r="194" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -6265,35 +6255,35 @@
         <v>590</v>
       </c>
       <c r="C194" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D194" s="4" t="s">
         <v>591</v>
       </c>
-      <c r="D194" s="4" t="s">
+      <c r="E194" s="5" t="s">
         <v>592</v>
-      </c>
-      <c r="E194" s="4" t="s">
-        <v>590</v>
       </c>
     </row>
     <row r="195" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A195" s="4" t="s">
+        <v>589</v>
+      </c>
+      <c r="B195" s="4" t="s">
         <v>593</v>
-      </c>
-      <c r="B195" s="4" t="s">
-        <v>594</v>
       </c>
       <c r="C195" s="4" t="s">
         <v>25</v>
       </c>
       <c r="D195" s="4" t="s">
+        <v>594</v>
+      </c>
+      <c r="E195" s="5" t="s">
         <v>595</v>
-      </c>
-      <c r="E195" s="5" t="s">
-        <v>596</v>
       </c>
     </row>
     <row r="196" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A196" s="4" t="s">
-        <v>593</v>
+        <v>596</v>
       </c>
       <c r="B196" s="4" t="s">
         <v>597</v>
@@ -6315,27 +6305,27 @@
       <c r="B197" s="4" t="s">
         <v>601</v>
       </c>
-      <c r="C197" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D197" s="4" t="s">
+      <c r="C197" s="5" t="s">
         <v>602</v>
       </c>
+      <c r="D197" s="5" t="s">
+        <v>603</v>
+      </c>
       <c r="E197" s="5" t="s">
-        <v>603</v>
+        <v>604</v>
       </c>
     </row>
     <row r="198" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A198" s="4" t="s">
-        <v>604</v>
+        <v>605</v>
       </c>
       <c r="B198" s="4" t="s">
-        <v>605</v>
-      </c>
-      <c r="C198" s="5" t="s">
         <v>606</v>
       </c>
-      <c r="D198" s="5" t="s">
+      <c r="C198" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D198" s="4" t="s">
         <v>607</v>
       </c>
       <c r="E198" s="5" t="s">
@@ -6344,104 +6334,87 @@
     </row>
     <row r="199" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A199" s="4" t="s">
+        <v>605</v>
+      </c>
+      <c r="B199" s="4" t="s">
         <v>609</v>
-      </c>
-      <c r="B199" s="4" t="s">
-        <v>610</v>
       </c>
       <c r="C199" s="4" t="s">
         <v>25</v>
       </c>
       <c r="D199" s="4" t="s">
+        <v>610</v>
+      </c>
+      <c r="E199" s="5" t="s">
         <v>611</v>
-      </c>
-      <c r="E199" s="5" t="s">
-        <v>612</v>
       </c>
     </row>
     <row r="200" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A200" s="4" t="s">
-        <v>609</v>
+        <v>605</v>
       </c>
       <c r="B200" s="4" t="s">
+        <v>612</v>
+      </c>
+      <c r="C200" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D200" s="4" t="s">
         <v>613</v>
       </c>
-      <c r="C200" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D200" s="4" t="s">
+      <c r="E200" s="5" t="s">
         <v>614</v>
-      </c>
-      <c r="E200" s="5" t="s">
-        <v>615</v>
       </c>
     </row>
     <row r="201" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A201" s="4" t="s">
-        <v>609</v>
+        <v>615</v>
       </c>
       <c r="B201" s="4" t="s">
+        <v>606</v>
+      </c>
+      <c r="C201" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D201" s="4" t="s">
         <v>616</v>
       </c>
-      <c r="C201" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D201" s="4" t="s">
+      <c r="E201" s="5" t="s">
         <v>617</v>
-      </c>
-      <c r="E201" s="5" t="s">
-        <v>618</v>
       </c>
     </row>
     <row r="202" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A202" s="4" t="s">
-        <v>619</v>
+        <v>615</v>
       </c>
       <c r="B202" s="4" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="C202" s="4" t="s">
         <v>25</v>
       </c>
       <c r="D202" s="4" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
       <c r="E202" s="5" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
     </row>
     <row r="203" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A203" s="4" t="s">
-        <v>619</v>
+        <v>615</v>
       </c>
       <c r="B203" s="4" t="s">
-        <v>613</v>
+        <v>620</v>
       </c>
       <c r="C203" s="4" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="D203" s="4" t="s">
+        <v>621</v>
+      </c>
+      <c r="E203" s="5" t="s">
         <v>622</v>
-      </c>
-      <c r="E203" s="5" t="s">
-        <v>623</v>
-      </c>
-    </row>
-    <row r="204" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A204" s="4" t="s">
-        <v>619</v>
-      </c>
-      <c r="B204" s="4" t="s">
-        <v>624</v>
-      </c>
-      <c r="C204" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D204" s="4" t="s">
-        <v>625</v>
-      </c>
-      <c r="E204" s="5" t="s">
-        <v>626</v>
       </c>
     </row>
   </sheetData>
@@ -6454,7 +6427,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
       <selection activeCell="A2" sqref="A2"/>
       <selection pane="bottomLeft" activeCell="E1" sqref="A1:XFD1048576"/>
@@ -6478,7 +6451,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>636</v>
+        <v>632</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>2</v>
@@ -6492,50 +6465,50 @@
         <v>73</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>627</v>
+        <v>623</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>628</v>
+        <v>624</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>629</v>
+        <v>625</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>630</v>
+        <v>626</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>631</v>
+        <v>627</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>632</v>
+        <v>628</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>633</v>
+        <v>629</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>25</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>634</v>
+        <v>630</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>635</v>
+        <v>631</v>
       </c>
     </row>
   </sheetData>

</xml_diff>